<commit_message>
- Add readmes - Body movement
</commit_message>
<xml_diff>
--- a/Body-movement/homework.xlsx
+++ b/Body-movement/homework.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Daniil\Projects\lbsu-modeling-tasks\Body-movement\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14C313AC-180F-4488-BA7E-85F78F023529}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{183DC5FC-19F9-4BA6-9C37-10B5381C8063}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-60" yWindow="-60" windowWidth="21720" windowHeight="12900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="з. 1" sheetId="1" r:id="rId1"/>
@@ -343,21 +343,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -368,9 +359,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
@@ -387,8 +375,19 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -12258,7 +12257,7 @@
   <dimension ref="A1:J56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -12269,53 +12268,53 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="5"/>
-      <c r="E1" s="1" t="s">
+      <c r="B1" s="15"/>
+      <c r="C1" s="16"/>
+      <c r="E1" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
     </row>
     <row r="2" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="5"/>
-      <c r="E2" s="15" t="s">
+      <c r="B2" s="15"/>
+      <c r="C2" s="16"/>
+      <c r="E2" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="15" t="s">
+      <c r="F2" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="15" t="s">
+      <c r="G2" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="15" t="s">
+      <c r="H2" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="15" t="s">
+      <c r="I2" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="J2" s="15" t="s">
+      <c r="J2" s="11" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A3" s="6">
+      <c r="A3" s="3">
         <v>30</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="8"/>
+      <c r="C3" s="5"/>
       <c r="E3" s="2">
         <v>0</v>
       </c>
@@ -12339,13 +12338,13 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A4" s="9">
+      <c r="A4" s="6">
         <v>60</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="11"/>
+      <c r="C4" s="7"/>
       <c r="E4" s="2">
         <f>E3+$A$5</f>
         <v>0.1</v>
@@ -12372,13 +12371,13 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A5" s="9">
+      <c r="A5" s="6">
         <v>0.1</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="11"/>
+      <c r="C5" s="7"/>
       <c r="E5" s="2">
         <f t="shared" ref="E5:E56" si="0">E4+$A$5</f>
         <v>0.2</v>
@@ -12405,13 +12404,13 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A6" s="9">
+      <c r="A6" s="6">
         <v>0.05</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="11"/>
+      <c r="C6" s="7"/>
       <c r="E6" s="2">
         <f t="shared" si="0"/>
         <v>0.30000000000000004</v>
@@ -12438,13 +12437,13 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A7" s="9">
+      <c r="A7" s="6">
         <v>2600</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="7" t="s">
         <v>9</v>
       </c>
       <c r="E7" s="2">
@@ -12473,13 +12472,13 @@
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A8" s="9">
+      <c r="A8" s="6">
         <v>1.2050000000000001</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="11"/>
+      <c r="C8" s="7"/>
       <c r="E8" s="2">
         <f t="shared" si="0"/>
         <v>0.5</v>
@@ -12506,13 +12505,13 @@
       </c>
     </row>
     <row r="9" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A9" s="12">
+      <c r="A9" s="8">
         <v>1.8099999999999999E-5</v>
       </c>
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="14"/>
+      <c r="C9" s="10"/>
       <c r="E9" s="2">
         <f t="shared" si="0"/>
         <v>0.6</v>
@@ -13786,53 +13785,53 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="5"/>
-      <c r="E1" s="1" t="s">
+      <c r="B1" s="15"/>
+      <c r="C1" s="16"/>
+      <c r="E1" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
     </row>
     <row r="2" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="5"/>
-      <c r="E2" s="15" t="s">
+      <c r="B2" s="15"/>
+      <c r="C2" s="16"/>
+      <c r="E2" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="15" t="s">
+      <c r="F2" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="15" t="s">
+      <c r="G2" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="15" t="s">
+      <c r="H2" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="15" t="s">
+      <c r="I2" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="J2" s="15" t="s">
+      <c r="J2" s="11" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A3" s="6">
+      <c r="A3" s="3">
         <v>30</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="8"/>
+      <c r="C3" s="5"/>
       <c r="E3" s="2">
         <v>0</v>
       </c>
@@ -13856,13 +13855,13 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A4" s="9">
+      <c r="A4" s="6">
         <v>60</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="11"/>
+      <c r="C4" s="7"/>
       <c r="E4" s="2">
         <f>E3+$A$5</f>
         <v>0.1</v>
@@ -13889,13 +13888,13 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A5" s="9">
+      <c r="A5" s="6">
         <v>0.1</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="11"/>
+      <c r="C5" s="7"/>
       <c r="E5" s="2">
         <f t="shared" ref="E5:E56" si="0">E4+$A$5</f>
         <v>0.2</v>
@@ -13922,13 +13921,13 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A6" s="9">
+      <c r="A6" s="6">
         <v>0.05</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="11"/>
+      <c r="C6" s="7"/>
       <c r="E6" s="2">
         <f t="shared" si="0"/>
         <v>0.30000000000000004</v>
@@ -13955,13 +13954,13 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A7" s="9">
+      <c r="A7" s="6">
         <v>2600</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="7" t="s">
         <v>9</v>
       </c>
       <c r="E7" s="2">
@@ -13990,13 +13989,13 @@
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A8" s="9">
+      <c r="A8" s="6">
         <v>0</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="11"/>
+      <c r="C8" s="7"/>
       <c r="E8" s="2">
         <f t="shared" si="0"/>
         <v>0.5</v>
@@ -14023,13 +14022,13 @@
       </c>
     </row>
     <row r="9" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A9" s="12">
+      <c r="A9" s="8">
         <v>0</v>
       </c>
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="14"/>
+      <c r="C9" s="10"/>
       <c r="E9" s="2">
         <f t="shared" si="0"/>
         <v>0.6</v>
@@ -15746,53 +15745,53 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="5"/>
-      <c r="E1" s="1" t="s">
+      <c r="B1" s="15"/>
+      <c r="C1" s="16"/>
+      <c r="E1" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
     </row>
     <row r="2" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="5"/>
-      <c r="E2" s="15" t="s">
+      <c r="B2" s="15"/>
+      <c r="C2" s="16"/>
+      <c r="E2" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="15" t="s">
+      <c r="F2" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="15" t="s">
+      <c r="G2" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="15" t="s">
+      <c r="H2" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="15" t="s">
+      <c r="I2" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="J2" s="15" t="s">
+      <c r="J2" s="11" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A3" s="6">
+      <c r="A3" s="3">
         <v>30</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="8"/>
+      <c r="C3" s="5"/>
       <c r="E3" s="2">
         <v>0</v>
       </c>
@@ -15816,13 +15815,13 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A4" s="9">
+      <c r="A4" s="6">
         <v>60</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="11"/>
+      <c r="C4" s="7"/>
       <c r="E4" s="2">
         <f>E3+$A$5</f>
         <v>0.1</v>
@@ -15849,13 +15848,13 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A5" s="9">
+      <c r="A5" s="6">
         <v>0.1</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="11"/>
+      <c r="C5" s="7"/>
       <c r="E5" s="2">
         <f t="shared" ref="E5:E20" si="0">E4+$A$5</f>
         <v>0.2</v>
@@ -15882,13 +15881,13 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A6" s="9">
+      <c r="A6" s="6">
         <v>0.05</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="11"/>
+      <c r="C6" s="7"/>
       <c r="E6" s="2">
         <f t="shared" si="0"/>
         <v>0.30000000000000004</v>
@@ -15915,13 +15914,13 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A7" s="9">
+      <c r="A7" s="6">
         <v>25</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="7" t="s">
         <v>17</v>
       </c>
       <c r="E7" s="2">
@@ -15950,13 +15949,13 @@
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A8" s="9">
+      <c r="A8" s="6">
         <v>1.2050000000000001</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="11"/>
+      <c r="C8" s="7"/>
       <c r="E8" s="2">
         <f t="shared" si="0"/>
         <v>0.5</v>
@@ -15983,13 +15982,13 @@
       </c>
     </row>
     <row r="9" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A9" s="12">
+      <c r="A9" s="8">
         <v>1.8099999999999999E-5</v>
       </c>
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="14"/>
+      <c r="C9" s="10"/>
       <c r="E9" s="2">
         <f t="shared" si="0"/>
         <v>0.6</v>
@@ -16548,10 +16547,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFBB4F95-2F9F-4659-8B59-A25B815879E9}">
-  <dimension ref="A1:J86"/>
+  <dimension ref="A1:J58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="O20" sqref="O20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -16561,53 +16560,53 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="5"/>
-      <c r="E1" s="1" t="s">
+      <c r="B1" s="15"/>
+      <c r="C1" s="16"/>
+      <c r="E1" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
     </row>
     <row r="2" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="5"/>
-      <c r="E2" s="15" t="s">
+      <c r="B2" s="15"/>
+      <c r="C2" s="16"/>
+      <c r="E2" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="15" t="s">
+      <c r="F2" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="15" t="s">
+      <c r="G2" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="15" t="s">
+      <c r="H2" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="15" t="s">
+      <c r="I2" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="J2" s="15" t="s">
+      <c r="J2" s="11" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A3" s="6">
+      <c r="A3" s="3">
         <v>30</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="8"/>
+      <c r="C3" s="5"/>
       <c r="E3" s="2">
         <v>0</v>
       </c>
@@ -16631,13 +16630,13 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A4" s="9">
+      <c r="A4" s="6">
         <v>60</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="11"/>
+      <c r="C4" s="7"/>
       <c r="E4" s="2">
         <f>E3+$A$5</f>
         <v>0.1</v>
@@ -16664,13 +16663,13 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A5" s="9">
+      <c r="A5" s="6">
         <v>0.1</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="11"/>
+      <c r="C5" s="7"/>
       <c r="E5" s="2">
         <f t="shared" ref="E5:E42" si="0">E4+$A$5</f>
         <v>0.2</v>
@@ -16697,13 +16696,13 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A6" s="9">
+      <c r="A6" s="6">
         <v>0.05</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="11"/>
+      <c r="C6" s="7"/>
       <c r="E6" s="2">
         <f t="shared" si="0"/>
         <v>0.30000000000000004</v>
@@ -16730,13 +16729,13 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A7" s="9">
+      <c r="A7" s="6">
         <v>25</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="7" t="s">
         <v>17</v>
       </c>
       <c r="E7" s="2">
@@ -16765,13 +16764,13 @@
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A8" s="9">
+      <c r="A8" s="6">
         <v>0</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="11"/>
+      <c r="C8" s="7"/>
       <c r="E8" s="2">
         <f t="shared" si="0"/>
         <v>0.5</v>
@@ -16798,13 +16797,13 @@
       </c>
     </row>
     <row r="9" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A9" s="12">
+      <c r="A9" s="8">
         <v>0</v>
       </c>
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="14"/>
+      <c r="C9" s="10"/>
       <c r="E9" s="2">
         <f t="shared" si="0"/>
         <v>0.6</v>
@@ -17690,27 +17689,27 @@
     </row>
     <row r="43" spans="5:10" x14ac:dyDescent="0.45">
       <c r="E43" s="2">
-        <f t="shared" ref="E43:E69" si="6">E42+$A$5</f>
+        <f t="shared" ref="E43:E57" si="6">E42+$A$5</f>
         <v>4.0000000000000018</v>
       </c>
       <c r="F43" s="2">
-        <f t="shared" ref="F43:F69" si="7">IF(J42 &lt; 0, 0, (1-H42*$A$5)*F42)</f>
+        <f t="shared" ref="F43:F57" si="7">IF(J42 &lt; 0, 0, (1-H42*$A$5)*F42)</f>
         <v>15.000000000000004</v>
       </c>
       <c r="G43" s="2">
-        <f t="shared" ref="G43:G69" si="8">($A$8/$A$7-1)*9.81*$A$5+(1-H42*$A$5)*G42</f>
+        <f t="shared" ref="G43:G57" si="8">($A$8/$A$7-1)*9.81*$A$5+(1-H42*$A$5)*G42</f>
         <v>-13.259237886466858</v>
       </c>
       <c r="H43" s="2">
-        <f t="shared" ref="H43:H69" si="9">(4.5*$A$9/$A$6+0.15*$A$8*SQRT(F43^2+G43^2))/($A$7*$A$6)</f>
+        <f t="shared" ref="H43:H57" si="9">(4.5*$A$9/$A$6+0.15*$A$8*SQRT(F43^2+G43^2))/($A$7*$A$6)</f>
         <v>0</v>
       </c>
       <c r="I43" s="2">
-        <f t="shared" ref="I43:I69" si="10">I42+IF($F43=0,0,F42*$A$5)</f>
+        <f t="shared" ref="I43:I57" si="10">I42+IF($F43=0,0,F42*$A$5)</f>
         <v>60.000000000000007</v>
       </c>
       <c r="J43" s="2">
-        <f t="shared" ref="J43:J69" si="11">J42+IF($F43=0,0,G42*$A$5)</f>
+        <f t="shared" ref="J43:J57" si="11">J42+IF($F43=0,0,G42*$A$5)</f>
         <v>27.405048454132572</v>
       </c>
     </row>
@@ -18053,262 +18052,38 @@
       </c>
     </row>
     <row r="57" spans="5:10" x14ac:dyDescent="0.45">
-      <c r="E57" s="16">
+      <c r="E57" s="12">
         <f t="shared" si="6"/>
         <v>5.3999999999999968</v>
       </c>
-      <c r="F57" s="16">
+      <c r="F57" s="12">
         <f t="shared" si="7"/>
         <v>15.000000000000004</v>
       </c>
-      <c r="G57" s="16">
+      <c r="G57" s="12">
         <f t="shared" si="8"/>
         <v>-26.993237886466876</v>
       </c>
-      <c r="H57" s="16">
+      <c r="H57" s="12">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="I57" s="16">
+      <c r="I57" s="12">
         <f t="shared" si="10"/>
         <v>81.000000000000014</v>
       </c>
-      <c r="J57" s="16">
+      <c r="J57" s="12">
         <f t="shared" si="11"/>
         <v>-8.4984586921040606E-2</v>
       </c>
     </row>
     <row r="58" spans="5:10" x14ac:dyDescent="0.45">
-      <c r="E58" s="18"/>
-      <c r="F58" s="18"/>
-      <c r="G58" s="18"/>
-      <c r="H58" s="18"/>
-      <c r="I58" s="18"/>
-      <c r="J58" s="18"/>
-    </row>
-    <row r="59" spans="5:10" x14ac:dyDescent="0.45">
-      <c r="E59" s="17"/>
-      <c r="F59" s="17"/>
-      <c r="G59" s="17"/>
-      <c r="H59" s="17"/>
-      <c r="I59" s="17"/>
-      <c r="J59" s="17"/>
-    </row>
-    <row r="60" spans="5:10" x14ac:dyDescent="0.45">
-      <c r="E60" s="17"/>
-      <c r="F60" s="17"/>
-      <c r="G60" s="17"/>
-      <c r="H60" s="17"/>
-      <c r="I60" s="17"/>
-      <c r="J60" s="17"/>
-    </row>
-    <row r="61" spans="5:10" x14ac:dyDescent="0.45">
-      <c r="E61" s="17"/>
-      <c r="F61" s="17"/>
-      <c r="G61" s="17"/>
-      <c r="H61" s="17"/>
-      <c r="I61" s="17"/>
-      <c r="J61" s="17"/>
-    </row>
-    <row r="62" spans="5:10" x14ac:dyDescent="0.45">
-      <c r="E62" s="17"/>
-      <c r="F62" s="17"/>
-      <c r="G62" s="17"/>
-      <c r="H62" s="17"/>
-      <c r="I62" s="17"/>
-      <c r="J62" s="17"/>
-    </row>
-    <row r="63" spans="5:10" x14ac:dyDescent="0.45">
-      <c r="E63" s="17"/>
-      <c r="F63" s="17"/>
-      <c r="G63" s="17"/>
-      <c r="H63" s="17"/>
-      <c r="I63" s="17"/>
-      <c r="J63" s="17"/>
-    </row>
-    <row r="64" spans="5:10" x14ac:dyDescent="0.45">
-      <c r="E64" s="17"/>
-      <c r="F64" s="17"/>
-      <c r="G64" s="17"/>
-      <c r="H64" s="17"/>
-      <c r="I64" s="17"/>
-      <c r="J64" s="17"/>
-    </row>
-    <row r="65" spans="5:10" x14ac:dyDescent="0.45">
-      <c r="E65" s="17"/>
-      <c r="F65" s="17"/>
-      <c r="G65" s="17"/>
-      <c r="H65" s="17"/>
-      <c r="I65" s="17"/>
-      <c r="J65" s="17"/>
-    </row>
-    <row r="66" spans="5:10" x14ac:dyDescent="0.45">
-      <c r="E66" s="17"/>
-      <c r="F66" s="17"/>
-      <c r="G66" s="17"/>
-      <c r="H66" s="17"/>
-      <c r="I66" s="17"/>
-      <c r="J66" s="17"/>
-    </row>
-    <row r="67" spans="5:10" x14ac:dyDescent="0.45">
-      <c r="E67" s="17"/>
-      <c r="F67" s="17"/>
-      <c r="G67" s="17"/>
-      <c r="H67" s="17"/>
-      <c r="I67" s="17"/>
-      <c r="J67" s="17"/>
-    </row>
-    <row r="68" spans="5:10" x14ac:dyDescent="0.45">
-      <c r="E68" s="17"/>
-      <c r="F68" s="17"/>
-      <c r="G68" s="17"/>
-      <c r="H68" s="17"/>
-      <c r="I68" s="17"/>
-      <c r="J68" s="17"/>
-    </row>
-    <row r="69" spans="5:10" x14ac:dyDescent="0.45">
-      <c r="E69" s="17"/>
-      <c r="F69" s="17"/>
-      <c r="G69" s="17"/>
-      <c r="H69" s="17"/>
-      <c r="I69" s="17"/>
-      <c r="J69" s="17"/>
-    </row>
-    <row r="70" spans="5:10" x14ac:dyDescent="0.45">
-      <c r="E70" s="17"/>
-      <c r="F70" s="17"/>
-      <c r="G70" s="17"/>
-      <c r="H70" s="17"/>
-      <c r="I70" s="17"/>
-      <c r="J70" s="17"/>
-    </row>
-    <row r="71" spans="5:10" x14ac:dyDescent="0.45">
-      <c r="E71" s="17"/>
-      <c r="F71" s="17"/>
-      <c r="G71" s="17"/>
-      <c r="H71" s="17"/>
-      <c r="I71" s="17"/>
-      <c r="J71" s="17"/>
-    </row>
-    <row r="72" spans="5:10" x14ac:dyDescent="0.45">
-      <c r="E72" s="17"/>
-      <c r="F72" s="17"/>
-      <c r="G72" s="17"/>
-      <c r="H72" s="17"/>
-      <c r="I72" s="17"/>
-      <c r="J72" s="17"/>
-    </row>
-    <row r="73" spans="5:10" x14ac:dyDescent="0.45">
-      <c r="E73" s="17"/>
-      <c r="F73" s="17"/>
-      <c r="G73" s="17"/>
-      <c r="H73" s="17"/>
-      <c r="I73" s="17"/>
-      <c r="J73" s="17"/>
-    </row>
-    <row r="74" spans="5:10" x14ac:dyDescent="0.45">
-      <c r="E74" s="17"/>
-      <c r="F74" s="17"/>
-      <c r="G74" s="17"/>
-      <c r="H74" s="17"/>
-      <c r="I74" s="17"/>
-      <c r="J74" s="17"/>
-    </row>
-    <row r="75" spans="5:10" x14ac:dyDescent="0.45">
-      <c r="E75" s="17"/>
-      <c r="F75" s="17"/>
-      <c r="G75" s="17"/>
-      <c r="H75" s="17"/>
-      <c r="I75" s="17"/>
-      <c r="J75" s="17"/>
-    </row>
-    <row r="76" spans="5:10" x14ac:dyDescent="0.45">
-      <c r="E76" s="17"/>
-      <c r="F76" s="17"/>
-      <c r="G76" s="17"/>
-      <c r="H76" s="17"/>
-      <c r="I76" s="17"/>
-      <c r="J76" s="17"/>
-    </row>
-    <row r="77" spans="5:10" x14ac:dyDescent="0.45">
-      <c r="E77" s="17"/>
-      <c r="F77" s="17"/>
-      <c r="G77" s="17"/>
-      <c r="H77" s="17"/>
-      <c r="I77" s="17"/>
-      <c r="J77" s="17"/>
-    </row>
-    <row r="78" spans="5:10" x14ac:dyDescent="0.45">
-      <c r="E78" s="17"/>
-      <c r="F78" s="17"/>
-      <c r="G78" s="17"/>
-      <c r="H78" s="17"/>
-      <c r="I78" s="17"/>
-      <c r="J78" s="17"/>
-    </row>
-    <row r="79" spans="5:10" x14ac:dyDescent="0.45">
-      <c r="E79" s="17"/>
-      <c r="F79" s="17"/>
-      <c r="G79" s="17"/>
-      <c r="H79" s="17"/>
-      <c r="I79" s="17"/>
-      <c r="J79" s="17"/>
-    </row>
-    <row r="80" spans="5:10" x14ac:dyDescent="0.45">
-      <c r="E80" s="17"/>
-      <c r="F80" s="17"/>
-      <c r="G80" s="17"/>
-      <c r="H80" s="17"/>
-      <c r="I80" s="17"/>
-      <c r="J80" s="17"/>
-    </row>
-    <row r="81" spans="5:10" x14ac:dyDescent="0.45">
-      <c r="E81" s="17"/>
-      <c r="F81" s="17"/>
-      <c r="G81" s="17"/>
-      <c r="H81" s="17"/>
-      <c r="I81" s="17"/>
-      <c r="J81" s="17"/>
-    </row>
-    <row r="82" spans="5:10" x14ac:dyDescent="0.45">
-      <c r="E82" s="17"/>
-      <c r="F82" s="17"/>
-      <c r="G82" s="17"/>
-      <c r="H82" s="17"/>
-      <c r="I82" s="17"/>
-      <c r="J82" s="17"/>
-    </row>
-    <row r="83" spans="5:10" x14ac:dyDescent="0.45">
-      <c r="E83" s="17"/>
-      <c r="F83" s="17"/>
-      <c r="G83" s="17"/>
-      <c r="H83" s="17"/>
-      <c r="I83" s="17"/>
-      <c r="J83" s="17"/>
-    </row>
-    <row r="84" spans="5:10" x14ac:dyDescent="0.45">
-      <c r="E84" s="17"/>
-      <c r="F84" s="17"/>
-      <c r="G84" s="17"/>
-      <c r="H84" s="17"/>
-      <c r="I84" s="17"/>
-      <c r="J84" s="17"/>
-    </row>
-    <row r="85" spans="5:10" x14ac:dyDescent="0.45">
-      <c r="E85" s="17"/>
-      <c r="F85" s="17"/>
-      <c r="G85" s="17"/>
-      <c r="H85" s="17"/>
-      <c r="I85" s="17"/>
-      <c r="J85" s="17"/>
-    </row>
-    <row r="86" spans="5:10" x14ac:dyDescent="0.45">
-      <c r="E86" s="17"/>
-      <c r="F86" s="17"/>
-      <c r="G86" s="17"/>
-      <c r="H86" s="17"/>
-      <c r="I86" s="17"/>
-      <c r="J86" s="17"/>
+      <c r="E58" s="13"/>
+      <c r="F58" s="13"/>
+      <c r="G58" s="13"/>
+      <c r="H58" s="13"/>
+      <c r="I58" s="13"/>
+      <c r="J58" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -18323,7 +18098,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{737AF652-E887-4511-942F-801E59B0D82E}">
-  <dimension ref="A1:J61"/>
+  <dimension ref="A1:J51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E1" sqref="E1:J4"/>
@@ -18336,53 +18111,53 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="5"/>
-      <c r="E1" s="1" t="s">
+      <c r="B1" s="15"/>
+      <c r="C1" s="16"/>
+      <c r="E1" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
     </row>
     <row r="2" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="5"/>
-      <c r="E2" s="15" t="s">
+      <c r="B2" s="15"/>
+      <c r="C2" s="16"/>
+      <c r="E2" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="15" t="s">
+      <c r="F2" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="15" t="s">
+      <c r="G2" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="15" t="s">
+      <c r="H2" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="15" t="s">
+      <c r="I2" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="J2" s="15" t="s">
+      <c r="J2" s="11" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A3" s="6">
+      <c r="A3" s="3">
         <v>0.5</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="8"/>
+      <c r="C3" s="5"/>
       <c r="E3" s="2">
         <v>0</v>
       </c>
@@ -18406,13 +18181,13 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A4" s="9">
+      <c r="A4" s="6">
         <v>0</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="11"/>
+      <c r="C4" s="7"/>
       <c r="E4" s="2">
         <f>E3+$A$5</f>
         <v>0.1</v>
@@ -18439,13 +18214,13 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A5" s="9">
+      <c r="A5" s="6">
         <v>0.1</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="11"/>
+      <c r="C5" s="7"/>
       <c r="E5" s="2">
         <f t="shared" ref="E5:E38" si="0">E4+$A$5</f>
         <v>0.2</v>
@@ -18472,13 +18247,13 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A6" s="9">
+      <c r="A6" s="6">
         <v>0.05</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="11"/>
+      <c r="C6" s="7"/>
       <c r="E6" s="2">
         <f t="shared" si="0"/>
         <v>0.30000000000000004</v>
@@ -18505,13 +18280,13 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A7" s="9">
+      <c r="A7" s="6">
         <v>2600</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="7" t="s">
         <v>9</v>
       </c>
       <c r="E7" s="2">
@@ -18540,13 +18315,13 @@
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A8" s="9">
+      <c r="A8" s="6">
         <v>997</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="11"/>
+      <c r="C8" s="7"/>
       <c r="E8" s="2">
         <f t="shared" si="0"/>
         <v>0.5</v>
@@ -18573,13 +18348,13 @@
       </c>
     </row>
     <row r="9" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A9" s="12">
+      <c r="A9" s="8">
         <v>0.01</v>
       </c>
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="14"/>
+      <c r="C9" s="10"/>
       <c r="E9" s="2">
         <f t="shared" si="0"/>
         <v>0.6</v>
@@ -19387,27 +19162,27 @@
     </row>
     <row r="40" spans="5:10" x14ac:dyDescent="0.45">
       <c r="E40" s="2">
-        <f t="shared" ref="E40:E61" si="6">E39+$A$5</f>
+        <f t="shared" ref="E40:E50" si="6">E39+$A$5</f>
         <v>3.700000000000002</v>
       </c>
       <c r="F40" s="2">
-        <f t="shared" ref="F40:F61" si="7">IF(J39 &lt; 0, 0, (1-H39*$A$5)*F39)</f>
+        <f t="shared" ref="F40:F50" si="7">IF(J39 &lt; 0, 0, (1-H39*$A$5)*F39)</f>
         <v>1.3483130174764137E-5</v>
       </c>
       <c r="G40" s="2">
-        <f t="shared" ref="G40:G61" si="8">($A$8/$A$7-1)*9.81*$A$5+(1-H39*$A$5)*G39</f>
+        <f t="shared" ref="G40:G50" si="8">($A$8/$A$7-1)*9.81*$A$5+(1-H39*$A$5)*G39</f>
         <v>-2.2899348888843325</v>
       </c>
       <c r="H40" s="2">
-        <f t="shared" ref="H40:H61" si="9">(4.5*$A$9/$A$6+0.15*$A$8*SQRT(F40^2+G40^2))/($A$7*$A$6)</f>
+        <f t="shared" ref="H40:H50" si="9">(4.5*$A$9/$A$6+0.15*$A$8*SQRT(F40^2+G40^2))/($A$7*$A$6)</f>
         <v>2.641228943373755</v>
       </c>
       <c r="I40" s="2">
-        <f t="shared" ref="I40:I61" si="10">I39+IF($F40=0,0,F39*$A$5)</f>
+        <f t="shared" ref="I40:I50" si="10">I39+IF($F40=0,0,F39*$A$5)</f>
         <v>0.29767339300444673</v>
       </c>
       <c r="J40" s="2">
-        <f t="shared" ref="J40:J61" si="11">J39+IF($F40=0,0,G39*$A$5)</f>
+        <f t="shared" ref="J40:J50" si="11">J39+IF($F40=0,0,G39*$A$5)</f>
         <v>2.1885518106295496</v>
       </c>
     </row>
@@ -19646,118 +19421,38 @@
       </c>
     </row>
     <row r="50" spans="5:10" x14ac:dyDescent="0.45">
-      <c r="E50" s="16">
+      <c r="E50" s="12">
         <f t="shared" si="6"/>
         <v>4.6999999999999993</v>
       </c>
-      <c r="F50" s="16">
+      <c r="F50" s="12">
         <f t="shared" si="7"/>
         <v>6.2783228217767728E-7</v>
       </c>
-      <c r="G50" s="16">
+      <c r="G50" s="12">
         <f t="shared" si="8"/>
         <v>-2.2899348890421285</v>
       </c>
-      <c r="H50" s="16">
+      <c r="H50" s="12">
         <f t="shared" si="9"/>
         <v>2.6412289435097165</v>
       </c>
-      <c r="I50" s="16">
+      <c r="I50" s="12">
         <f t="shared" si="10"/>
         <v>0.29767826016975801</v>
       </c>
-      <c r="J50" s="16">
+      <c r="J50" s="12">
         <f t="shared" si="11"/>
         <v>-0.10138307837868632</v>
       </c>
     </row>
     <row r="51" spans="5:10" x14ac:dyDescent="0.45">
-      <c r="E51" s="18"/>
-      <c r="F51" s="18"/>
-      <c r="G51" s="18"/>
-      <c r="H51" s="18"/>
-      <c r="I51" s="18"/>
-      <c r="J51" s="18"/>
-    </row>
-    <row r="52" spans="5:10" x14ac:dyDescent="0.45">
-      <c r="E52" s="17"/>
-      <c r="F52" s="17"/>
-      <c r="G52" s="17"/>
-      <c r="H52" s="17"/>
-      <c r="I52" s="17"/>
-      <c r="J52" s="17"/>
-    </row>
-    <row r="53" spans="5:10" x14ac:dyDescent="0.45">
-      <c r="E53" s="17"/>
-      <c r="F53" s="17"/>
-      <c r="G53" s="17"/>
-      <c r="H53" s="17"/>
-      <c r="I53" s="17"/>
-      <c r="J53" s="17"/>
-    </row>
-    <row r="54" spans="5:10" x14ac:dyDescent="0.45">
-      <c r="E54" s="17"/>
-      <c r="F54" s="17"/>
-      <c r="G54" s="17"/>
-      <c r="H54" s="17"/>
-      <c r="I54" s="17"/>
-      <c r="J54" s="17"/>
-    </row>
-    <row r="55" spans="5:10" x14ac:dyDescent="0.45">
-      <c r="E55" s="17"/>
-      <c r="F55" s="17"/>
-      <c r="G55" s="17"/>
-      <c r="H55" s="17"/>
-      <c r="I55" s="17"/>
-      <c r="J55" s="17"/>
-    </row>
-    <row r="56" spans="5:10" x14ac:dyDescent="0.45">
-      <c r="E56" s="17"/>
-      <c r="F56" s="17"/>
-      <c r="G56" s="17"/>
-      <c r="H56" s="17"/>
-      <c r="I56" s="17"/>
-      <c r="J56" s="17"/>
-    </row>
-    <row r="57" spans="5:10" x14ac:dyDescent="0.45">
-      <c r="E57" s="17"/>
-      <c r="F57" s="17"/>
-      <c r="G57" s="17"/>
-      <c r="H57" s="17"/>
-      <c r="I57" s="17"/>
-      <c r="J57" s="17"/>
-    </row>
-    <row r="58" spans="5:10" x14ac:dyDescent="0.45">
-      <c r="E58" s="17"/>
-      <c r="F58" s="17"/>
-      <c r="G58" s="17"/>
-      <c r="H58" s="17"/>
-      <c r="I58" s="17"/>
-      <c r="J58" s="17"/>
-    </row>
-    <row r="59" spans="5:10" x14ac:dyDescent="0.45">
-      <c r="E59" s="17"/>
-      <c r="F59" s="17"/>
-      <c r="G59" s="17"/>
-      <c r="H59" s="17"/>
-      <c r="I59" s="17"/>
-      <c r="J59" s="17"/>
-    </row>
-    <row r="60" spans="5:10" x14ac:dyDescent="0.45">
-      <c r="E60" s="17"/>
-      <c r="F60" s="17"/>
-      <c r="G60" s="17"/>
-      <c r="H60" s="17"/>
-      <c r="I60" s="17"/>
-      <c r="J60" s="17"/>
-    </row>
-    <row r="61" spans="5:10" x14ac:dyDescent="0.45">
-      <c r="E61" s="17"/>
-      <c r="F61" s="17"/>
-      <c r="G61" s="17"/>
-      <c r="H61" s="17"/>
-      <c r="I61" s="17"/>
-      <c r="J61" s="17"/>
+      <c r="E51" s="13"/>
+      <c r="F51" s="13"/>
+      <c r="G51" s="13"/>
+      <c r="H51" s="13"/>
+      <c r="I51" s="13"/>
+      <c r="J51" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -19773,9 +19468,9 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A61EA9E-1693-49DD-9896-F0156B72DD92}">
-  <dimension ref="A1:J50"/>
+  <dimension ref="A1:J30"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
@@ -19786,53 +19481,53 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="5"/>
-      <c r="E1" s="1" t="s">
+      <c r="B1" s="15"/>
+      <c r="C1" s="16"/>
+      <c r="E1" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
     </row>
     <row r="2" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="5"/>
-      <c r="E2" s="15" t="s">
+      <c r="B2" s="15"/>
+      <c r="C2" s="16"/>
+      <c r="E2" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="15" t="s">
+      <c r="F2" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="15" t="s">
+      <c r="G2" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="15" t="s">
+      <c r="H2" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="15" t="s">
+      <c r="I2" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="J2" s="15" t="s">
+      <c r="J2" s="11" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A3" s="6">
+      <c r="A3" s="3">
         <v>0.5</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="8"/>
+      <c r="C3" s="5"/>
       <c r="E3" s="2">
         <v>0</v>
       </c>
@@ -19856,13 +19551,13 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A4" s="9">
+      <c r="A4" s="6">
         <v>0</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="11"/>
+      <c r="C4" s="7"/>
       <c r="E4" s="2">
         <f>E3+$A$5</f>
         <v>0.1</v>
@@ -19889,31 +19584,31 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A5" s="9">
+      <c r="A5" s="6">
         <v>0.1</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="11"/>
+      <c r="C5" s="7"/>
       <c r="E5" s="2">
-        <f t="shared" ref="E5:E38" si="0">E4+$A$5</f>
+        <f t="shared" ref="E5:E29" si="0">E4+$A$5</f>
         <v>0.2</v>
       </c>
       <c r="F5" s="2">
-        <f t="shared" ref="F5:F38" si="1">IF(J4 &lt; 0, 0, (1-H4*$A$5)*F4)</f>
+        <f t="shared" ref="F5:F29" si="1">IF(J4 &lt; 0, 0, (1-H4*$A$5)*F4)</f>
         <v>0.4718747260957129</v>
       </c>
       <c r="G5" s="2">
-        <f t="shared" ref="G5:G38" si="2">($A$8/$A$7-1)*9.81*$A$5+(1-H4*$A$5)*G4</f>
+        <f t="shared" ref="G5:G29" si="2">($A$8/$A$7-1)*9.81*$A$5+(1-H4*$A$5)*G4</f>
         <v>-1.6811095841431969</v>
       </c>
       <c r="H5" s="2">
-        <f t="shared" ref="H5:H38" si="3">(4.5*$A$9/$A$6+0.15*$A$8*SQRT(F5^2+G5^2))/($A$7*$A$6)</f>
+        <f t="shared" ref="H5:H29" si="3">(4.5*$A$9/$A$6+0.15*$A$8*SQRT(F5^2+G5^2))/($A$7*$A$6)</f>
         <v>0.66588629349351214</v>
       </c>
       <c r="I5" s="2">
-        <f t="shared" ref="I5:J38" si="4">I4+IF($F5=0,0,F4*$A$5)</f>
+        <f t="shared" ref="I5:J29" si="4">I4+IF($F5=0,0,F4*$A$5)</f>
         <v>9.9038437102922497E-2</v>
       </c>
       <c r="J5" s="2">
@@ -19922,13 +19617,13 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A6" s="9">
+      <c r="A6" s="6">
         <v>0.05</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="11"/>
+      <c r="C6" s="7"/>
       <c r="E6" s="2">
         <f t="shared" si="0"/>
         <v>0.30000000000000004</v>
@@ -19955,13 +19650,13 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A7" s="9">
+      <c r="A7" s="6">
         <v>7870</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="7" t="s">
         <v>19</v>
       </c>
       <c r="E7" s="2">
@@ -19990,13 +19685,13 @@
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A8" s="9">
+      <c r="A8" s="6">
         <v>997</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="11"/>
+      <c r="C8" s="7"/>
       <c r="E8" s="2">
         <f t="shared" si="0"/>
         <v>0.5</v>
@@ -20023,13 +19718,13 @@
       </c>
     </row>
     <row r="9" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A9" s="12">
+      <c r="A9" s="8">
         <v>0.01</v>
       </c>
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="14"/>
+      <c r="C9" s="10"/>
       <c r="E9" s="2">
         <f t="shared" si="0"/>
         <v>0.6</v>
@@ -20550,198 +20245,38 @@
       </c>
     </row>
     <row r="29" spans="5:10" x14ac:dyDescent="0.45">
-      <c r="E29" s="16">
+      <c r="E29" s="12">
         <f t="shared" si="0"/>
         <v>2.600000000000001</v>
       </c>
-      <c r="F29" s="16">
+      <c r="F29" s="12">
         <f t="shared" si="1"/>
         <v>6.3247847956350205E-3</v>
       </c>
-      <c r="G29" s="16">
+      <c r="G29" s="12">
         <f t="shared" si="2"/>
         <v>-4.7447326706061181</v>
       </c>
-      <c r="H29" s="16">
+      <c r="H29" s="12">
         <f t="shared" si="3"/>
         <v>1.8055283388001526</v>
       </c>
-      <c r="I29" s="16">
+      <c r="I29" s="12">
         <f t="shared" si="4"/>
         <v>0.4421679775711751</v>
       </c>
-      <c r="J29" s="16">
+      <c r="J29" s="12">
         <f t="shared" si="4"/>
         <v>-0.40597768208698864</v>
       </c>
     </row>
     <row r="30" spans="5:10" x14ac:dyDescent="0.45">
-      <c r="E30" s="18"/>
-      <c r="F30" s="18"/>
-      <c r="G30" s="18"/>
-      <c r="H30" s="18"/>
-      <c r="I30" s="18"/>
-      <c r="J30" s="18"/>
-    </row>
-    <row r="31" spans="5:10" x14ac:dyDescent="0.45">
-      <c r="E31" s="17"/>
-      <c r="F31" s="17"/>
-      <c r="G31" s="17"/>
-      <c r="H31" s="17"/>
-      <c r="I31" s="17"/>
-      <c r="J31" s="17"/>
-    </row>
-    <row r="32" spans="5:10" x14ac:dyDescent="0.45">
-      <c r="E32" s="17"/>
-      <c r="F32" s="17"/>
-      <c r="G32" s="17"/>
-      <c r="H32" s="17"/>
-      <c r="I32" s="17"/>
-      <c r="J32" s="17"/>
-    </row>
-    <row r="33" spans="5:10" x14ac:dyDescent="0.45">
-      <c r="E33" s="17"/>
-      <c r="F33" s="17"/>
-      <c r="G33" s="17"/>
-      <c r="H33" s="17"/>
-      <c r="I33" s="17"/>
-      <c r="J33" s="17"/>
-    </row>
-    <row r="34" spans="5:10" x14ac:dyDescent="0.45">
-      <c r="E34" s="17"/>
-      <c r="F34" s="17"/>
-      <c r="G34" s="17"/>
-      <c r="H34" s="17"/>
-      <c r="I34" s="17"/>
-      <c r="J34" s="17"/>
-    </row>
-    <row r="35" spans="5:10" x14ac:dyDescent="0.45">
-      <c r="E35" s="17"/>
-      <c r="F35" s="17"/>
-      <c r="G35" s="17"/>
-      <c r="H35" s="17"/>
-      <c r="I35" s="17"/>
-      <c r="J35" s="17"/>
-    </row>
-    <row r="36" spans="5:10" x14ac:dyDescent="0.45">
-      <c r="E36" s="17"/>
-      <c r="F36" s="17"/>
-      <c r="G36" s="17"/>
-      <c r="H36" s="17"/>
-      <c r="I36" s="17"/>
-      <c r="J36" s="17"/>
-    </row>
-    <row r="37" spans="5:10" x14ac:dyDescent="0.45">
-      <c r="E37" s="17"/>
-      <c r="F37" s="17"/>
-      <c r="G37" s="17"/>
-      <c r="H37" s="17"/>
-      <c r="I37" s="17"/>
-      <c r="J37" s="17"/>
-    </row>
-    <row r="38" spans="5:10" x14ac:dyDescent="0.45">
-      <c r="E38" s="17"/>
-      <c r="F38" s="17"/>
-      <c r="G38" s="17"/>
-      <c r="H38" s="17"/>
-      <c r="I38" s="17"/>
-      <c r="J38" s="17"/>
-    </row>
-    <row r="39" spans="5:10" x14ac:dyDescent="0.45">
-      <c r="E39" s="17"/>
-      <c r="F39" s="17"/>
-      <c r="G39" s="17"/>
-      <c r="H39" s="17"/>
-      <c r="I39" s="17"/>
-      <c r="J39" s="17"/>
-    </row>
-    <row r="40" spans="5:10" x14ac:dyDescent="0.45">
-      <c r="E40" s="17"/>
-      <c r="F40" s="17"/>
-      <c r="G40" s="17"/>
-      <c r="H40" s="17"/>
-      <c r="I40" s="17"/>
-      <c r="J40" s="17"/>
-    </row>
-    <row r="41" spans="5:10" x14ac:dyDescent="0.45">
-      <c r="E41" s="17"/>
-      <c r="F41" s="17"/>
-      <c r="G41" s="17"/>
-      <c r="H41" s="17"/>
-      <c r="I41" s="17"/>
-      <c r="J41" s="17"/>
-    </row>
-    <row r="42" spans="5:10" x14ac:dyDescent="0.45">
-      <c r="E42" s="17"/>
-      <c r="F42" s="17"/>
-      <c r="G42" s="17"/>
-      <c r="H42" s="17"/>
-      <c r="I42" s="17"/>
-      <c r="J42" s="17"/>
-    </row>
-    <row r="43" spans="5:10" x14ac:dyDescent="0.45">
-      <c r="E43" s="17"/>
-      <c r="F43" s="17"/>
-      <c r="G43" s="17"/>
-      <c r="H43" s="17"/>
-      <c r="I43" s="17"/>
-      <c r="J43" s="17"/>
-    </row>
-    <row r="44" spans="5:10" x14ac:dyDescent="0.45">
-      <c r="E44" s="17"/>
-      <c r="F44" s="17"/>
-      <c r="G44" s="17"/>
-      <c r="H44" s="17"/>
-      <c r="I44" s="17"/>
-      <c r="J44" s="17"/>
-    </row>
-    <row r="45" spans="5:10" x14ac:dyDescent="0.45">
-      <c r="E45" s="17"/>
-      <c r="F45" s="17"/>
-      <c r="G45" s="17"/>
-      <c r="H45" s="17"/>
-      <c r="I45" s="17"/>
-      <c r="J45" s="17"/>
-    </row>
-    <row r="46" spans="5:10" x14ac:dyDescent="0.45">
-      <c r="E46" s="17"/>
-      <c r="F46" s="17"/>
-      <c r="G46" s="17"/>
-      <c r="H46" s="17"/>
-      <c r="I46" s="17"/>
-      <c r="J46" s="17"/>
-    </row>
-    <row r="47" spans="5:10" x14ac:dyDescent="0.45">
-      <c r="E47" s="17"/>
-      <c r="F47" s="17"/>
-      <c r="G47" s="17"/>
-      <c r="H47" s="17"/>
-      <c r="I47" s="17"/>
-      <c r="J47" s="17"/>
-    </row>
-    <row r="48" spans="5:10" x14ac:dyDescent="0.45">
-      <c r="E48" s="17"/>
-      <c r="F48" s="17"/>
-      <c r="G48" s="17"/>
-      <c r="H48" s="17"/>
-      <c r="I48" s="17"/>
-      <c r="J48" s="17"/>
-    </row>
-    <row r="49" spans="5:10" x14ac:dyDescent="0.45">
-      <c r="E49" s="17"/>
-      <c r="F49" s="17"/>
-      <c r="G49" s="17"/>
-      <c r="H49" s="17"/>
-      <c r="I49" s="17"/>
-      <c r="J49" s="17"/>
-    </row>
-    <row r="50" spans="5:10" x14ac:dyDescent="0.45">
-      <c r="E50" s="17"/>
-      <c r="F50" s="17"/>
-      <c r="G50" s="17"/>
-      <c r="H50" s="17"/>
-      <c r="I50" s="17"/>
-      <c r="J50" s="17"/>
+      <c r="E30" s="13"/>
+      <c r="F30" s="13"/>
+      <c r="G30" s="13"/>
+      <c r="H30" s="13"/>
+      <c r="I30" s="13"/>
+      <c r="J30" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -20769,53 +20304,53 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="5"/>
-      <c r="E1" s="1" t="s">
+      <c r="B1" s="15"/>
+      <c r="C1" s="16"/>
+      <c r="E1" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
     </row>
     <row r="2" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="5"/>
-      <c r="E2" s="15" t="s">
+      <c r="B2" s="15"/>
+      <c r="C2" s="16"/>
+      <c r="E2" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="15" t="s">
+      <c r="F2" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="15" t="s">
+      <c r="G2" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="15" t="s">
+      <c r="H2" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="15" t="s">
+      <c r="I2" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="J2" s="15" t="s">
+      <c r="J2" s="11" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A3" s="6">
+      <c r="A3" s="3">
         <v>0.5</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="8"/>
+      <c r="C3" s="5"/>
       <c r="E3" s="2">
         <v>0</v>
       </c>
@@ -20839,13 +20374,13 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A4" s="9">
+      <c r="A4" s="6">
         <v>0</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="11"/>
+      <c r="C4" s="7"/>
       <c r="E4" s="2">
         <f>E3+$A$5</f>
         <v>1E-3</v>
@@ -20872,13 +20407,13 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A5" s="9">
+      <c r="A5" s="6">
         <v>1E-3</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="11"/>
+      <c r="C5" s="7"/>
       <c r="E5" s="2">
         <f t="shared" ref="E5:E68" si="0">E4+$A$5</f>
         <v>2E-3</v>
@@ -20905,13 +20440,13 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A6" s="9">
+      <c r="A6" s="6">
         <v>0.05</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="11"/>
+      <c r="C6" s="7"/>
       <c r="E6" s="2">
         <f t="shared" si="0"/>
         <v>3.0000000000000001E-3</v>
@@ -20938,13 +20473,13 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A7" s="9">
+      <c r="A7" s="6">
         <v>25</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="7" t="s">
         <v>17</v>
       </c>
       <c r="E7" s="2">
@@ -20973,13 +20508,13 @@
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A8" s="9">
+      <c r="A8" s="6">
         <v>997</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="11"/>
+      <c r="C8" s="7"/>
       <c r="E8" s="2">
         <f t="shared" si="0"/>
         <v>5.0000000000000001E-3</v>
@@ -21006,13 +20541,13 @@
       </c>
     </row>
     <row r="9" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A9" s="12">
+      <c r="A9" s="8">
         <v>0.01</v>
       </c>
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="14"/>
+      <c r="C9" s="10"/>
       <c r="E9" s="2">
         <f t="shared" si="0"/>
         <v>6.0000000000000001E-3</v>
@@ -26176,7 +25711,7 @@
   <dimension ref="A1:J320"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J320" sqref="I3:J320"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -26187,53 +25722,53 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="5"/>
-      <c r="E1" s="1" t="s">
+      <c r="B1" s="15"/>
+      <c r="C1" s="16"/>
+      <c r="E1" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
     </row>
     <row r="2" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="5"/>
-      <c r="E2" s="15" t="s">
+      <c r="B2" s="15"/>
+      <c r="C2" s="16"/>
+      <c r="E2" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="15" t="s">
+      <c r="F2" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="15" t="s">
+      <c r="G2" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="15" t="s">
+      <c r="H2" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="15" t="s">
+      <c r="I2" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="J2" s="15" t="s">
+      <c r="J2" s="11" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A3" s="6">
+      <c r="A3" s="3">
         <v>0.5</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="8"/>
+      <c r="C3" s="5"/>
       <c r="E3" s="2">
         <v>0</v>
       </c>
@@ -26257,13 +25792,13 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A4" s="9">
+      <c r="A4" s="6">
         <v>0</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="11"/>
+      <c r="C4" s="7"/>
       <c r="E4" s="2">
         <f>E3+$A$5</f>
         <v>1E-3</v>
@@ -26290,13 +25825,13 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A5" s="9">
+      <c r="A5" s="6">
         <v>1E-3</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="11"/>
+      <c r="C5" s="7"/>
       <c r="E5" s="2">
         <f t="shared" ref="E5:E68" si="0">E4+$A$5</f>
         <v>2E-3</v>
@@ -26323,13 +25858,13 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A6" s="9">
+      <c r="A6" s="6">
         <v>0.05</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="11"/>
+      <c r="C6" s="7"/>
       <c r="E6" s="2">
         <f t="shared" si="0"/>
         <v>3.0000000000000001E-3</v>
@@ -26356,13 +25891,13 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A7" s="9">
+      <c r="A7" s="6">
         <v>450</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="7" t="s">
         <v>20</v>
       </c>
       <c r="E7" s="2">
@@ -26391,13 +25926,13 @@
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A8" s="9">
+      <c r="A8" s="6">
         <v>997</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="11"/>
+      <c r="C8" s="7"/>
       <c r="E8" s="2">
         <f t="shared" si="0"/>
         <v>5.0000000000000001E-3</v>
@@ -26424,13 +25959,13 @@
       </c>
     </row>
     <row r="9" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A9" s="12">
+      <c r="A9" s="8">
         <v>0.01</v>
       </c>
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="14"/>
+      <c r="C9" s="10"/>
       <c r="E9" s="2">
         <f t="shared" si="0"/>
         <v>6.0000000000000001E-3</v>

</xml_diff>